<commit_message>
AGC012A 1st Finish !!!
</commit_message>
<xml_diff>
--- a/atcoder/AtCoder回答実績.xlsx
+++ b/atcoder/AtCoder回答実績.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\yamanaka\cppprog\atcoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FA60C1-CEC4-44B6-BDC3-31F8EABCE0E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C661F2C2-B753-434C-8D76-B702F6CB2E21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BeginnersSelection" sheetId="1" r:id="rId1"/>
@@ -1604,8 +1604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2410,6 +2410,9 @@
       <c r="D30" s="8">
         <v>43951</v>
       </c>
+      <c r="E30" s="8">
+        <v>43954</v>
+      </c>
       <c r="J30" s="8">
         <v>43613</v>
       </c>
@@ -2424,6 +2427,9 @@
       <c r="C31" s="8">
         <v>43951</v>
       </c>
+      <c r="D31" s="8">
+        <v>43954</v>
+      </c>
       <c r="J31" s="8">
         <v>43618</v>
       </c>
@@ -2434,6 +2440,9 @@
     <row r="32" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>121</v>
+      </c>
+      <c r="C32" s="8">
+        <v>43958</v>
       </c>
       <c r="J32" s="8">
         <v>43624</v>

</xml_diff>